<commit_message>
MongoDB Integration - Part 1
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Desktop\china-taste\china-taste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C90525-F3B6-4A1E-B4B6-B60F24BCD9E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8D11A6-49C7-4482-B0F5-68E755730F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4060" xr2:uid="{0A59E1DF-BFF7-454A-BB24-E9C2AA1C05AF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -87,9 +87,6 @@
     <t>https://crackstation.net/hashing-security.htm</t>
   </si>
   <si>
-    <t>Add "Profile" page*</t>
-  </si>
-  <si>
     <t>Add "Past Orders" page*</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>Standardize button ID tags</t>
+  </si>
+  <si>
+    <t>Add "Profile" page</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5FC0C-F12A-465A-8993-7A253663FE8A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +529,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
@@ -538,12 +538,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -552,12 +552,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -566,12 +566,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -579,11 +579,13 @@
       <c r="C5" s="2">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -595,7 +597,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -619,7 +621,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -657,7 +659,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -666,12 +668,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -680,12 +682,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -781,7 +783,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -829,7 +831,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -841,7 +843,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2">
         <v>8</v>
@@ -852,7 +854,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
@@ -863,7 +865,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
Bcrypt integration for secure password hashing
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Desktop\china-taste\china-taste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8D11A6-49C7-4482-B0F5-68E755730F0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DACEB-FE65-4015-A01D-B183DACD0AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4060" xr2:uid="{0A59E1DF-BFF7-454A-BB24-E9C2AA1C05AF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>https://crackstation.net/hashing-security.htm</t>
@@ -501,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5FC0C-F12A-465A-8993-7A253663FE8A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +526,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
@@ -538,12 +535,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -552,12 +549,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -566,12 +563,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -580,12 +577,12 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -597,7 +594,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -621,7 +618,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -630,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -659,7 +656,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -668,12 +665,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -682,12 +679,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -707,7 +704,9 @@
       <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -767,7 +766,9 @@
       <c r="C20" s="2">
         <v>3</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -783,7 +784,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -831,7 +832,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -843,7 +844,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
         <v>8</v>
@@ -854,7 +855,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
@@ -865,7 +866,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2">
         <v>5</v>
@@ -876,7 +877,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bcrypt integration for secure password hashing - Part 2
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Desktop\china-taste\china-taste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DACEB-FE65-4015-A01D-B183DACD0AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45637B-2951-4130-A60B-15566B293A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4060" xr2:uid="{0A59E1DF-BFF7-454A-BB24-E9C2AA1C05AF}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>https://crackstation.net/hashing-security.htm</t>
-  </si>
-  <si>
     <t>Add "Past Orders" page*</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Add "Profile" page</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5FC0C-F12A-465A-8993-7A253663FE8A}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +526,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
@@ -535,12 +535,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -549,12 +549,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -563,12 +563,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -577,12 +577,12 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -627,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -656,7 +656,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -665,12 +665,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -679,12 +679,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -692,7 +692,9 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -705,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -767,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -784,7 +786,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -832,7 +834,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -844,7 +846,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
         <v>8</v>
@@ -855,7 +857,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
@@ -866,18 +868,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
         <v>5</v>
       </c>
       <c r="C29" s="2">
         <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Bcrypt integration for secure password hashing - Part 2"
This reverts commit e5ae757049cd5f35f4cb9e0f9f839eafb4922c88.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Desktop\china-taste\china-taste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45637B-2951-4130-A60B-15566B293A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DACEB-FE65-4015-A01D-B183DACD0AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4060" xr2:uid="{0A59E1DF-BFF7-454A-BB24-E9C2AA1C05AF}"/>
   </bookViews>
@@ -81,6 +81,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>https://crackstation.net/hashing-security.htm</t>
+  </si>
+  <si>
     <t>Add "Past Orders" page*</t>
   </si>
   <si>
@@ -130,9 +133,6 @@
   </si>
   <si>
     <t>Add "Profile" page</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5FC0C-F12A-465A-8993-7A253663FE8A}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +526,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
@@ -535,12 +535,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -549,12 +549,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -563,12 +563,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -577,12 +577,12 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -627,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -656,7 +656,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -665,12 +665,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -679,12 +679,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -692,9 +692,7 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -707,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -769,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -786,7 +784,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -834,7 +832,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -846,7 +844,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
         <v>8</v>
@@ -857,7 +855,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
@@ -868,13 +866,18 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2">
         <v>5</v>
       </c>
       <c r="C29" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Bcrypt integration for secure password hashing - Part 2""
This reverts commit 46afd97712b8f1128822ec8231e5fcc18896a76d.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Desktop\china-taste\china-taste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6DACEB-FE65-4015-A01D-B183DACD0AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD45637B-2951-4130-A60B-15566B293A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4060" xr2:uid="{0A59E1DF-BFF7-454A-BB24-E9C2AA1C05AF}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>https://crackstation.net/hashing-security.htm</t>
-  </si>
-  <si>
     <t>Add "Past Orders" page*</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Add "Profile" page</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5FC0C-F12A-465A-8993-7A253663FE8A}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +526,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
@@ -535,12 +535,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -549,12 +549,12 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -563,12 +563,12 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
@@ -577,12 +577,12 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <v>5</v>
@@ -627,7 +627,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -656,7 +656,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -665,12 +665,12 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -679,12 +679,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -692,7 +692,9 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -705,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -767,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -784,7 +786,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -832,7 +834,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -844,7 +846,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
         <v>8</v>
@@ -855,7 +857,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
         <v>8</v>
@@ -866,18 +868,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
         <v>5</v>
       </c>
       <c r="C29" s="2">
         <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>